<commit_message>
More WIP on Main User Screen
</commit_message>
<xml_diff>
--- a/Documentation/Navigation_18DEC20.xlsx
+++ b/Documentation/Navigation_18DEC20.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\asl\ASL4321 Project\ASL4321_Display_Demo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDFB390-3E28-4CB9-A4F8-509B104F09DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FDBBA0-A3C2-4ADF-8D5C-E042232F9865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings and Navigation" sheetId="1" r:id="rId1"/>
     <sheet name="Programming" sheetId="2" r:id="rId2"/>
-    <sheet name="User Screen" sheetId="3" r:id="rId3"/>
+    <sheet name="Newer Main Screen" sheetId="4" r:id="rId3"/>
+    <sheet name="User Screen" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -557,6 +558,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -573,9 +577,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1733,6 +1734,1048 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>75162</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{567EFBC0-6713-4A6B-8A04-13B18E9829A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="761999"/>
+          <a:ext cx="2457449" cy="1408663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>70457</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{247C30BF-E836-44F4-AF29-8539C2D3DE22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="2667000"/>
+          <a:ext cx="2447925" cy="1403957"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>83932</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E2107A-5D82-48B0-91D1-A3039DE3A614}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6134101" y="971550"/>
+          <a:ext cx="2457450" cy="1398382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>11334</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF870777-04D6-4F46-9037-5E445955D190}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9134476" y="971550"/>
+          <a:ext cx="2459258" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>77336</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53ECC7BE-8C71-4DFE-8440-DE0DD8127450}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12258676" y="962025"/>
+          <a:ext cx="2449060" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>42341</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE80CF09-2C4C-4AEE-94D7-AB17FE8B4D94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15278100" y="952500"/>
+          <a:ext cx="2442641" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>41827</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC09728A-35A9-453F-9766-DEAF4A5A3F0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18316575" y="962026"/>
+          <a:ext cx="2451652" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>597496</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5B22961-7096-43C1-B374-6DBD9EA8A0C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15240000" y="3057525"/>
+          <a:ext cx="2426296" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>68991</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4536A244-0E51-4C68-ABE7-4B247490E495}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15240000" y="5124450"/>
+          <a:ext cx="2447925" cy="1421541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>5625</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4E369F-AACA-4B06-85A7-A5020E7DE983}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15220950" y="7258050"/>
+          <a:ext cx="2463075" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133462</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>98771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>184496</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Arrow: Right 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695240F8-2BA8-46C1-8B74-6F68D3A520E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3791062" y="1241771"/>
+          <a:ext cx="2257314" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Long USER PORT SWITCH</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> press</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38212</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>136871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>32096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Arrow: Right 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038AE41E-7108-4EA2-8DE1-73A826324820}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8572612" y="1279871"/>
+          <a:ext cx="599963" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Long USER PORT SWITCH</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> press</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38212</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>13046</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Arrow: Right 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D77C8BD1-D56C-4A2D-8A17-DF0F573E2964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11620612" y="1260821"/>
+          <a:ext cx="599963" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Long USER PORT SWITCH</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> press</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>76312</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>136871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>32096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Arrow: Right 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31607B7F-8A0C-463D-907E-221264A2314E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14706712" y="1279871"/>
+          <a:ext cx="599963" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Long USER PORT SWITCH</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> press</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>342956</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>108352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>200081</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>41565</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Arrow: Right 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95A50C28-B5F7-4917-82C2-4E801615642A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="16078312" y="2508596"/>
+          <a:ext cx="695213" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Short</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>362006</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>79777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>219131</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12990</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Arrow: Right 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C57D764-67C9-4C9E-B052-11753CCA0A58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="16097362" y="4575521"/>
+          <a:ext cx="695213" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Short</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>362006</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>89302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>219131</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>22515</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Arrow: Right 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{198249A9-21B0-4BD1-A7F1-F139C4C24C34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="16097362" y="6680546"/>
+          <a:ext cx="695213" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Short</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>561630</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123065</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>418755</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88198</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Arrow: Right 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE7A1C82-279B-4A7C-BB41-007EEF1CDC25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18261064">
+          <a:off x="17195426" y="3872769"/>
+          <a:ext cx="3775133" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Long USER PORT SWITCH</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> press (TYPICAL)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>57262</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3521</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>89246</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Arrow: Right 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974BBD1E-F382-49C6-B340-0526E3A2B5F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17735662" y="1337021"/>
+          <a:ext cx="599963" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Long USER PORT SWITCH</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> press</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2982,10 +4025,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3042,18 +4085,18 @@
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -3102,22 +4145,22 @@
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22" t="s">
+      <c r="G5" s="23"/>
+      <c r="H5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="22"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="1" t="s">
         <v>5</v>
       </c>
@@ -3190,28 +4233,28 @@
     </row>
     <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -3241,14 +4284,14 @@
     </row>
     <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
       <c r="J8" s="5" t="s">
         <v>16</v>
       </c>
@@ -3274,14 +4317,14 @@
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
       <c r="J9" s="5" t="s">
         <v>18</v>
       </c>
@@ -3336,18 +4379,18 @@
     </row>
     <row r="11" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -3396,22 +4439,22 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="22"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="1" t="s">
         <v>5</v>
       </c>
@@ -3484,28 +4527,28 @@
     </row>
     <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="24" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -3535,14 +4578,14 @@
     </row>
     <row r="16" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
       <c r="J16" s="5" t="s">
         <v>16</v>
       </c>
@@ -3570,14 +4613,14 @@
     </row>
     <row r="17" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
       <c r="J17" s="5" t="s">
         <v>25</v>
       </c>
@@ -3605,14 +4648,14 @@
     </row>
     <row r="18" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
       <c r="J18" s="5" t="s">
         <v>27</v>
       </c>
@@ -3640,14 +4683,14 @@
     </row>
     <row r="19" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
       <c r="J19" s="5" t="s">
         <v>25</v>
       </c>
@@ -3704,18 +4747,18 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -3764,22 +4807,22 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22" t="s">
+      <c r="C23" s="23"/>
+      <c r="D23" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22" t="s">
+      <c r="E23" s="23"/>
+      <c r="F23" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22" t="s">
+      <c r="G23" s="23"/>
+      <c r="H23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="22"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="1" t="s">
         <v>5</v>
       </c>
@@ -4194,18 +5237,18 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -4254,22 +5297,22 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22" t="s">
+      <c r="C37" s="23"/>
+      <c r="D37" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22" t="s">
+      <c r="E37" s="23"/>
+      <c r="F37" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22" t="s">
+      <c r="G37" s="23"/>
+      <c r="H37" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="22"/>
+      <c r="I37" s="23"/>
       <c r="J37" s="1" t="s">
         <v>5</v>
       </c>
@@ -4342,28 +5385,28 @@
     </row>
     <row r="39" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H39" s="23" t="s">
+      <c r="H39" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I39" s="24" t="s">
         <v>47</v>
       </c>
       <c r="J39" s="8" t="s">
@@ -4391,14 +5434,14 @@
     </row>
     <row r="40" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
       <c r="J40" s="8" t="s">
         <v>27</v>
       </c>
@@ -4426,14 +5469,14 @@
     </row>
     <row r="41" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
       <c r="J41" s="8" t="s">
         <v>45</v>
       </c>
@@ -4459,18 +5502,18 @@
     </row>
     <row r="43" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -4519,22 +5562,22 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22" t="s">
+      <c r="C45" s="23"/>
+      <c r="D45" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22" t="s">
+      <c r="E45" s="23"/>
+      <c r="F45" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22" t="s">
+      <c r="G45" s="23"/>
+      <c r="H45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="22"/>
+      <c r="I45" s="23"/>
       <c r="J45" s="1" t="s">
         <v>5</v>
       </c>
@@ -4675,18 +5718,18 @@
     </row>
     <row r="50" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
@@ -4735,22 +5778,22 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22" t="s">
+      <c r="C52" s="23"/>
+      <c r="D52" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22" t="s">
+      <c r="E52" s="23"/>
+      <c r="F52" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22" t="s">
+      <c r="G52" s="23"/>
+      <c r="H52" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="22"/>
+      <c r="I52" s="23"/>
       <c r="J52" s="1" t="s">
         <v>5</v>
       </c>
@@ -4888,18 +5931,18 @@
     </row>
     <row r="57" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="22"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -4919,22 +5962,22 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22" t="s">
+      <c r="C58" s="23"/>
+      <c r="D58" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22" t="s">
+      <c r="E58" s="23"/>
+      <c r="F58" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22" t="s">
+      <c r="G58" s="23"/>
+      <c r="H58" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="22"/>
+      <c r="I58" s="23"/>
       <c r="J58" s="1" t="s">
         <v>5</v>
       </c>
@@ -5104,6 +6147,74 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="B57:K57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G25:G33"/>
+    <mergeCell ref="H25:H33"/>
+    <mergeCell ref="I25:I33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="D25:D33"/>
+    <mergeCell ref="E25:E33"/>
+    <mergeCell ref="F25:F33"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
     <mergeCell ref="G54:G55"/>
     <mergeCell ref="H54:H55"/>
     <mergeCell ref="I54:I55"/>
@@ -5120,74 +6231,6 @@
     <mergeCell ref="F54:F55"/>
     <mergeCell ref="I39:I41"/>
     <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="G25:G33"/>
-    <mergeCell ref="H25:H33"/>
-    <mergeCell ref="I25:I33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="D25:D33"/>
-    <mergeCell ref="E25:E33"/>
-    <mergeCell ref="F25:F33"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="B57:K57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5385,10 +6428,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2337612-48A8-46D0-AA61-2B18318E8B5B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>

</xml_diff>